<commit_message>
Add and modify column names in new tables
</commit_message>
<xml_diff>
--- a/data/TestData_10x_2024_12_16.xlsx
+++ b/data/TestData_10x_2024_12_16.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/developmentalneurobiology/core_operations/Bioinformatics/achroni/GitHub/sc-atac-seq/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72629E16-18A0-C44A-991C-A6585DB4CA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FB67F1-CA84-3C4F-BD12-ABB4F2A37C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25760" yWindow="-3120" windowWidth="25460" windowHeight="20720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,12 +41,6 @@
     <t>DYE</t>
   </si>
   <si>
-    <t>SRM #</t>
-  </si>
-  <si>
-    <t>SRM Sample #</t>
-  </si>
-  <si>
     <t>Kit</t>
   </si>
   <si>
@@ -243,6 +237,12 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>SRM_id</t>
+  </si>
+  <si>
+    <t>SRM_Sample_id</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -663,119 +663,119 @@
     <col min="7" max="7" width="28.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5">
         <v>277093</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5">
         <v>277093</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
         <v>277094</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
         <v>277094</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
         <v>180168</v>
@@ -784,42 +784,42 @@
         <v>1883579</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
         <v>1883580</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2">
         <v>180170</v>
@@ -828,42 +828,42 @@
         <v>1883583</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="2">
         <v>1883584</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2">
         <v>208969</v>
@@ -872,21 +872,21 @@
         <v>2089363</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2">
         <v>245789</v>
@@ -895,21 +895,21 @@
         <v>2294832</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2">
         <v>245789</v>
@@ -918,21 +918,21 @@
         <v>2294833</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2">
         <v>245789</v>
@@ -941,21 +941,21 @@
         <v>2294834</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2">
         <v>245790</v>
@@ -964,21 +964,21 @@
         <v>2294835</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2">
         <v>245790</v>
@@ -987,21 +987,21 @@
         <v>2294836</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2">
         <v>245790</v>
@@ -1010,21 +1010,21 @@
         <v>2294837</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2">
         <v>163737</v>
@@ -1033,21 +1033,21 @@
         <v>1883585</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C18" s="2">
         <v>163737</v>
@@ -1056,21 +1056,21 @@
         <v>1883586</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3">
         <v>157682</v>
@@ -1079,21 +1079,21 @@
         <v>1657575</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="2">
         <v>163737</v>
@@ -1102,21 +1102,21 @@
         <v>1721277</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2">
         <v>163734</v>
@@ -1125,63 +1125,63 @@
         <v>1721257</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2">
         <v>152367</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="2">
         <v>152367</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="3">
         <v>157682</v>
@@ -1190,21 +1190,21 @@
         <v>1657569</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" s="3">
         <v>157682</v>
@@ -1213,21 +1213,21 @@
         <v>1657570</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3">
         <v>157682</v>
@@ -1236,21 +1236,21 @@
         <v>1657571</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3">
         <v>157682</v>
@@ -1259,21 +1259,21 @@
         <v>1657572</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="3">
         <v>157684</v>
@@ -1282,21 +1282,21 @@
         <v>1657591</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" s="3">
         <v>157684</v>
@@ -1305,21 +1305,21 @@
         <v>1657592</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C30" s="3">
         <v>157684</v>
@@ -1328,21 +1328,21 @@
         <v>1657593</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="3">
         <v>157684</v>
@@ -1351,21 +1351,21 @@
         <v>1657594</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C32" s="2">
         <v>206690</v>
@@ -1374,21 +1374,21 @@
         <v>2074625</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C33" s="2">
         <v>206690</v>
@@ -1397,21 +1397,21 @@
         <v>2074626</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C34" s="2">
         <v>206686</v>
@@ -1420,13 +1420,13 @@
         <v>2074611</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>